<commit_message>
updated root path + SPL data
updated root path;
added SPL data from speaker experiments
</commit_message>
<xml_diff>
--- a/Data/Fig R4 Data_SB_AMP_THD_2022_01_2831.xlsx
+++ b/Data/Fig R4 Data_SB_AMP_THD_2022_01_2831.xlsx
@@ -31,6 +31,7 @@
     <sheet name="SB_AMP_THD+N_CHR_-30dBFS_8Ohms" sheetId="32" r:id="rId22"/>
     <sheet name="SB_AMP_THD+N_CHR_-40dBFS" sheetId="33" r:id="rId23"/>
     <sheet name="SB_AMP_THD+N_CHR_-40dBFS_8Ohms" sheetId="34" r:id="rId24"/>
+    <sheet name="SB_AMP_THD+N_CHR_-40dBFS_4Ohms" sheetId="38" r:id="rId25"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5674" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6190" uniqueCount="58">
   <si>
     <t>UPV SWEEP TRACE FILE</t>
   </si>
@@ -210,6 +211,12 @@
   </si>
   <si>
     <t>2 axis with %</t>
+  </si>
+  <si>
+    <t>R&amp;S UPP400 Serial no: 140002, 2022-4-2, 16:46:35</t>
+  </si>
+  <si>
+    <t>R&amp;S UPP400 Serial no: 140002, 2022-4-2, 16:38:56</t>
   </si>
 </sst>
 </file>
@@ -5315,6 +5322,782 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-FA8E-426F-AC1A-E37532732FF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:v>CHR_-40dBFS_4Ohms</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SB_AMP_THD+N_CHR_-40dBFS_4Ohms'!$A$17:$A$70</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.467869694219999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.051120943840004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.916344231159997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.255011558769993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.2871926885</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>115.26582642850001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>132.4816298678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>152.26874084240001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175.0112031447</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>201.15042034699999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>231.1937229088</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>265.72421484490002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>305.4120910661</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>351.02764504850001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>403.4562192944</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>463.71538875469997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>532.97471072320002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>612.57842452320006</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>704.07154155980004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>809.22983211539997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>930.09429089369996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1069.010750248</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1228.67540994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1412.1871670989999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1623.107762053</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1865.5309073870001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2144.1617419260001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2464.4081517660002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2832.4857307819998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3255.538417747</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3741.7771515119998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4300.6392353580004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4942.9715035890003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5681.2408454099996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6529.7761721099996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7505.0465238249999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8625.9807136060008</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9914.3347126869994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11395.11390747</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13097.058423709999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15053.20093743</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17301.50779906</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19885.6159142</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>22855.67968293</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>26269.34443583</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>30192.865259819999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>34702.392928929999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>39885.451898359999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45842.639047800003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>52689.576144760002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>60559.153922619997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>69604.111328350002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>80000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SB_AMP_THD+N_CHR_-40dBFS_4Ohms'!$B$17:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>-58.86832422378</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-58.845421105489997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-58.866549899600003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-58.905434206400002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-58.954890238510004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-58.905973251570003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-58.860162771239999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-58.981294452059998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-58.89541465792</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-58.88612540151</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-58.875707632290002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-58.919377735300003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-58.886262831019998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-58.849622717560003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-58.893899104239999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-58.919302130029997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-58.832125359880003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-58.856492201800002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-58.93686172196</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-58.870254753879998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-58.890530662659998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-58.88235843535</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-58.9948989512</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-58.922621120300001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-58.956441476560002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-59.041407487500003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-58.929823931850002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-58.809818281440002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-58.86013860245</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-58.936388750589998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-58.903401987670001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-58.94959052467</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-58.93063789456</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-58.908227694920001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-58.90190838174</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-58.947029944640001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-58.91921682281</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-58.930624470209999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-58.956429500500001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-58.97857133438</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-58.993085028979998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-58.884482172360002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-58.954894537400001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-58.964228736419997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-59.07153149637</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-59.133931924979997</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-59.25963780611</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-59.521359840640002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-59.704849681459997</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-60.140916850460002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-60.681313911140002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-60.666888976229998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-59.916402867670001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-58.112661602140001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B762-4BDA-A592-6726B3AF7F7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:v>CHR_-30dBFS_4Ohms</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SB_AMP_THD+N_CHR_-30dBFS_4Ohms'!$A$17:$A$70</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.467869694219999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.051120943840004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.916344231159997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.255011558769993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.2871926885</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>115.26582642850001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>132.4816298678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>152.26874084240001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175.0112031447</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>201.15042034699999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>231.1937229088</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>265.72421484490002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>305.4120910661</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>351.02764504850001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>403.4562192944</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>463.71538875469997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>532.97471072320002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>612.57842452320006</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>704.07154155980004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>809.22983211539997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>930.09429089369996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1069.010750248</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1228.67540994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1412.1871670989999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1623.107762053</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1865.5309073870001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2144.1617419260001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2464.4081517660002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2832.4857307819998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3255.538417747</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3741.7771515119998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4300.6392353580004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4942.9715035890003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5681.2408454099996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6529.7761721099996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7505.0465238249999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8625.9807136060008</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9914.3347126869994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11395.11390747</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13097.058423709999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15053.20093743</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17301.50779906</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19885.6159142</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>22855.67968293</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>26269.34443583</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>30192.865259819999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>34702.392928929999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>39885.451898359999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45842.639047800003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>52689.576144760002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>60559.153922619997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>69604.111328350002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>80000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SB_AMP_THD+N_CHR_-30dBFS_4Ohms'!$B$17:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>-69.034657681390001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-68.93152126951</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-68.964048098730004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-68.900009208049994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-69.00394811084</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-69.043502804010004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-68.935114415800001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-68.941653773740001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-68.889478386519997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-68.935134028419995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-68.955460431660001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-68.875090263640004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-68.972435605599998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-68.99041116107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-68.998823685310001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-68.853204856109997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-68.950137954170003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-68.921575866020007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-68.9453805303</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-69.017915570219998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-68.949060195290002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-68.872630550400004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-68.959232724670002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-68.991329093350004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-68.931431085100002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-68.962498537619993</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-68.934752622689999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-69.046906666230001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-68.908623224799996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-68.952272628469998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-68.973762046740006</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-68.880095189079995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-68.930227778930004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-68.986584987320001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-68.98417027587</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-68.998005719930006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-69.020651069630006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-69.127164764989999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-69.05456610105</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-69.087081332530005</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-69.063195128619995</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-69.099544647819997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-69.110365782049996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-68.983564894470007</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-69.112110290209998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-69.206859442899997</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-69.414719143379997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-69.556892957870005</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-69.944161269259993</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-70.137740290829996</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-70.509847889780005</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-70.547610430109998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-69.704240653629995</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-67.915524873039999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B762-4BDA-A592-6726B3AF7F7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10889,7 +11672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="W38:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
@@ -33977,14 +34760,1922 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection sqref="A1:K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>-140</v>
+      </c>
+      <c r="C9">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>80000</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-69.034657681390001</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F17" s="1">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-1.5768881475109999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>57.467869694219999</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-68.93152126951</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F18" s="1">
+        <v>57.467869694219999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-1.60175516834</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>66.051120943840004</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-68.964048098730004</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F19" s="1">
+        <v>66.051120943840004</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-1.6274119334099999</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>75.916344231159997</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-68.900009208049994</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F20" s="1">
+        <v>75.916344231159997</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-1.6373715092979999</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>87.255011558769993</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-69.00394811084</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F21" s="1">
+        <v>87.255011558769993</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-1.64825267263</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>100.2871926885</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-69.043502804010004</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F22" s="1">
+        <v>100.2871926885</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-1.649181031695</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>115.26582642850001</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-68.935114415800001</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F23" s="1">
+        <v>115.26582642850001</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-1.609930057898</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>132.4816298678</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-68.941653773740001</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F24" s="1">
+        <v>132.4816298678</v>
+      </c>
+      <c r="G24" s="1">
+        <v>-1.6346057361919999</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>152.26874084240001</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-68.889478386519997</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F25" s="1">
+        <v>152.26874084240001</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-1.6240759681550001</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>175.0112031447</v>
+      </c>
+      <c r="B26" s="1">
+        <v>-68.935134028419995</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F26" s="1">
+        <v>175.0112031447</v>
+      </c>
+      <c r="G26" s="1">
+        <v>-1.6119964034780001</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>201.15042034699999</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-68.955460431660001</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F27" s="1">
+        <v>201.15042034699999</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-1.6155323959100001</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>231.1937229088</v>
+      </c>
+      <c r="B28" s="1">
+        <v>-68.875090263640004</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F28" s="1">
+        <v>231.1937229088</v>
+      </c>
+      <c r="G28" s="1">
+        <v>-1.6468796989350001</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>265.72421484490002</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-68.972435605599998</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F29" s="1">
+        <v>265.72421484490002</v>
+      </c>
+      <c r="G29" s="1">
+        <v>-1.652580352238</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>305.4120910661</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-68.99041116107</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F30" s="1">
+        <v>305.4120910661</v>
+      </c>
+      <c r="G30" s="1">
+        <v>-1.5903413212299999</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>351.02764504850001</v>
+      </c>
+      <c r="B31" s="1">
+        <v>-68.998823685310001</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F31" s="1">
+        <v>351.02764504850001</v>
+      </c>
+      <c r="G31" s="1">
+        <v>-1.612168099617</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>403.4562192944</v>
+      </c>
+      <c r="B32" s="1">
+        <v>-68.853204856109997</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F32" s="1">
+        <v>403.4562192944</v>
+      </c>
+      <c r="G32" s="1">
+        <v>-1.615944105976</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>463.71538875469997</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-68.950137954170003</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F33" s="1">
+        <v>463.71538875469997</v>
+      </c>
+      <c r="G33" s="1">
+        <v>-1.591404861222</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>532.97471072320002</v>
+      </c>
+      <c r="B34" s="1">
+        <v>-68.921575866020007</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F34" s="1">
+        <v>532.97471072320002</v>
+      </c>
+      <c r="G34" s="1">
+        <v>-1.634208789256</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>612.57842452320006</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-68.9453805303</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F35" s="1">
+        <v>612.57842452320006</v>
+      </c>
+      <c r="G35" s="1">
+        <v>-1.65180603574</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>704.07154155980004</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-69.017915570219998</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F36" s="1">
+        <v>704.07154155980004</v>
+      </c>
+      <c r="G36" s="1">
+        <v>-1.611380413884</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>809.22983211539997</v>
+      </c>
+      <c r="B37" s="1">
+        <v>-68.949060195290002</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F37" s="1">
+        <v>809.22983211539997</v>
+      </c>
+      <c r="G37" s="1">
+        <v>-1.5910589477329999</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>930.09429089369996</v>
+      </c>
+      <c r="B38" s="1">
+        <v>-68.872630550400004</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F38" s="1">
+        <v>930.09429089369996</v>
+      </c>
+      <c r="G38" s="1">
+        <v>-1.607363846982</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1069.010750248</v>
+      </c>
+      <c r="B39" s="1">
+        <v>-68.959232724670002</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1069.010750248</v>
+      </c>
+      <c r="G39" s="1">
+        <v>-1.6089926522489999</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1228.67540994</v>
+      </c>
+      <c r="B40" s="1">
+        <v>-68.991329093350004</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1228.67540994</v>
+      </c>
+      <c r="G40" s="1">
+        <v>-1.6226901519700001</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>1412.1871670989999</v>
+      </c>
+      <c r="B41" s="1">
+        <v>-68.931431085100002</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1412.1871670989999</v>
+      </c>
+      <c r="G41" s="1">
+        <v>-1.6171504093769999</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1623.107762053</v>
+      </c>
+      <c r="B42" s="1">
+        <v>-68.962498537619993</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1623.107762053</v>
+      </c>
+      <c r="G42" s="1">
+        <v>-1.6223680574570001</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1865.5309073870001</v>
+      </c>
+      <c r="B43" s="1">
+        <v>-68.934752622689999</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1865.5309073870001</v>
+      </c>
+      <c r="G43" s="1">
+        <v>-1.623506963191</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2144.1617419260001</v>
+      </c>
+      <c r="B44" s="1">
+        <v>-69.046906666230001</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2144.1617419260001</v>
+      </c>
+      <c r="G44" s="1">
+        <v>-1.609881363712</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2464.4081517660002</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-68.908623224799996</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2464.4081517660002</v>
+      </c>
+      <c r="G45" s="1">
+        <v>-1.6157585423280001</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>2832.4857307819998</v>
+      </c>
+      <c r="B46" s="1">
+        <v>-68.952272628469998</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2832.4857307819998</v>
+      </c>
+      <c r="G46" s="1">
+        <v>-1.5844989026330001</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>3255.538417747</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-68.973762046740006</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3255.538417747</v>
+      </c>
+      <c r="G47" s="1">
+        <v>-1.5889010636630001</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>3741.7771515119998</v>
+      </c>
+      <c r="B48" s="1">
+        <v>-68.880095189079995</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3741.7771515119998</v>
+      </c>
+      <c r="G48" s="1">
+        <v>-1.6269022470950001</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>4300.6392353580004</v>
+      </c>
+      <c r="B49" s="1">
+        <v>-68.930227778930004</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F49" s="1">
+        <v>4300.6392353580004</v>
+      </c>
+      <c r="G49" s="1">
+        <v>-1.6144918957859999</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>4942.9715035890003</v>
+      </c>
+      <c r="B50" s="1">
+        <v>-68.986584987320001</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F50" s="1">
+        <v>4942.9715035890003</v>
+      </c>
+      <c r="G50" s="1">
+        <v>-1.6407750293309999</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>5681.2408454099996</v>
+      </c>
+      <c r="B51" s="1">
+        <v>-68.98417027587</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F51" s="1">
+        <v>5681.2408454099996</v>
+      </c>
+      <c r="G51" s="1">
+        <v>-1.5841886376080001</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>6529.7761721099996</v>
+      </c>
+      <c r="B52" s="1">
+        <v>-68.998005719930006</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F52" s="1">
+        <v>6529.7761721099996</v>
+      </c>
+      <c r="G52" s="1">
+        <v>-1.591142567256</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>7505.0465238249999</v>
+      </c>
+      <c r="B53" s="1">
+        <v>-69.020651069630006</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F53" s="1">
+        <v>7505.0465238249999</v>
+      </c>
+      <c r="G53" s="1">
+        <v>-1.6203461120289999</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>8625.9807136060008</v>
+      </c>
+      <c r="B54" s="1">
+        <v>-69.127164764989999</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F54" s="1">
+        <v>8625.9807136060008</v>
+      </c>
+      <c r="G54" s="1">
+        <v>-1.6448839654059999</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
+        <v>15</v>
+      </c>
+      <c r="J54" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>9914.3347126869994</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-69.05456610105</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F55" s="1">
+        <v>9914.3347126869994</v>
+      </c>
+      <c r="G55" s="1">
+        <v>-1.6252025530480001</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" t="s">
+        <v>15</v>
+      </c>
+      <c r="J55" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>11395.11390747</v>
+      </c>
+      <c r="B56" s="1">
+        <v>-69.087081332530005</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F56" s="1">
+        <v>11395.11390747</v>
+      </c>
+      <c r="G56" s="1">
+        <v>-1.5922674708190001</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>13097.058423709999</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-69.063195128619995</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F57" s="1">
+        <v>13097.058423709999</v>
+      </c>
+      <c r="G57" s="1">
+        <v>-1.641419401903</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>15053.20093743</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-69.099544647819997</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F58" s="1">
+        <v>15053.20093743</v>
+      </c>
+      <c r="G58" s="1">
+        <v>-1.5460902244270001</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>15</v>
+      </c>
+      <c r="J58" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>17301.50779906</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-69.110365782049996</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F59" s="1">
+        <v>17301.50779906</v>
+      </c>
+      <c r="G59" s="1">
+        <v>-1.588261628625</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J59" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>19885.6159142</v>
+      </c>
+      <c r="B60" s="1">
+        <v>-68.983564894470007</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F60" s="1">
+        <v>19885.6159142</v>
+      </c>
+      <c r="G60" s="1">
+        <v>-1.624269609205</v>
+      </c>
+      <c r="H60" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>22855.67968293</v>
+      </c>
+      <c r="B61" s="1">
+        <v>-69.112110290209998</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F61" s="1">
+        <v>22855.67968293</v>
+      </c>
+      <c r="G61" s="1">
+        <v>-1.7043864865089999</v>
+      </c>
+      <c r="H61" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" t="s">
+        <v>15</v>
+      </c>
+      <c r="J61" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>26269.34443583</v>
+      </c>
+      <c r="B62" s="1">
+        <v>-69.206859442899997</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F62" s="1">
+        <v>26269.34443583</v>
+      </c>
+      <c r="G62" s="1">
+        <v>-1.562153255003</v>
+      </c>
+      <c r="H62" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" t="s">
+        <v>15</v>
+      </c>
+      <c r="J62" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>30192.865259819999</v>
+      </c>
+      <c r="B63" s="1">
+        <v>-69.414719143379997</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F63" s="1">
+        <v>30192.865259819999</v>
+      </c>
+      <c r="G63" s="1">
+        <v>-1.5687593493409999</v>
+      </c>
+      <c r="H63" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>34702.392928929999</v>
+      </c>
+      <c r="B64" s="1">
+        <v>-69.556892957870005</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F64" s="1">
+        <v>34702.392928929999</v>
+      </c>
+      <c r="G64" s="1">
+        <v>-1.525411683445</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>39885.451898359999</v>
+      </c>
+      <c r="B65" s="1">
+        <v>-69.944161269259993</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F65" s="1">
+        <v>39885.451898359999</v>
+      </c>
+      <c r="G65" s="1">
+        <v>-1.6093644370569999</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" t="s">
+        <v>15</v>
+      </c>
+      <c r="J65" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>45842.639047800003</v>
+      </c>
+      <c r="B66" s="1">
+        <v>-70.137740290829996</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45842.639047800003</v>
+      </c>
+      <c r="G66" s="1">
+        <v>-1.6511760756110001</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" t="s">
+        <v>15</v>
+      </c>
+      <c r="J66" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>52689.576144760002</v>
+      </c>
+      <c r="B67" s="1">
+        <v>-70.509847889780005</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F67" s="1">
+        <v>52689.576144760002</v>
+      </c>
+      <c r="G67" s="1">
+        <v>-1.4975413688929999</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" t="s">
+        <v>15</v>
+      </c>
+      <c r="J67" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>60559.153922619997</v>
+      </c>
+      <c r="B68" s="1">
+        <v>-70.547610430109998</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F68" s="1">
+        <v>60559.153922619997</v>
+      </c>
+      <c r="G68" s="1">
+        <v>-1.5984232185759999</v>
+      </c>
+      <c r="H68" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" t="s">
+        <v>15</v>
+      </c>
+      <c r="J68" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>69604.111328350002</v>
+      </c>
+      <c r="B69" s="1">
+        <v>-69.704240653629995</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F69" s="1">
+        <v>69604.111328350002</v>
+      </c>
+      <c r="G69" s="1">
+        <v>-1.56459088688</v>
+      </c>
+      <c r="H69" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B70" s="1">
+        <v>-67.915524873039999</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F70" s="1">
+        <v>80000</v>
+      </c>
+      <c r="G70" s="1">
+        <v>-1.5855127386679999</v>
+      </c>
+      <c r="H70" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" t="s">
+        <v>15</v>
+      </c>
+      <c r="J70" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -39755,6 +42446,1928 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection sqref="A1:K70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>-140</v>
+      </c>
+      <c r="C9">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>80000</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-58.86832422378</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F17" s="1">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-1.6758521052690001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>57.467869694219999</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-58.845421105489997</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F18" s="1">
+        <v>57.467869694219999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-1.7014170949280001</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>66.051120943840004</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-58.866549899600003</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F19" s="1">
+        <v>66.051120943840004</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-1.6880638827859999</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>75.916344231159997</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-58.905434206400002</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F20" s="1">
+        <v>75.916344231159997</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-1.7052083533960001</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>87.255011558769993</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-58.954890238510004</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F21" s="1">
+        <v>87.255011558769993</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-1.725438253144</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>100.2871926885</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-58.905973251570003</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F22" s="1">
+        <v>100.2871926885</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-1.689643070197</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>115.26582642850001</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-58.860162771239999</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F23" s="1">
+        <v>115.26582642850001</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-1.666473687174</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>132.4816298678</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-58.981294452059998</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F24" s="1">
+        <v>132.4816298678</v>
+      </c>
+      <c r="G24" s="1">
+        <v>-1.656512244602</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>152.26874084240001</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-58.89541465792</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F25" s="1">
+        <v>152.26874084240001</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-1.651811510258</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>175.0112031447</v>
+      </c>
+      <c r="B26" s="1">
+        <v>-58.88612540151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F26" s="1">
+        <v>175.0112031447</v>
+      </c>
+      <c r="G26" s="1">
+        <v>-1.6391456416079999</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>201.15042034699999</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-58.875707632290002</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F27" s="1">
+        <v>201.15042034699999</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-1.6621132615900001</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>231.1937229088</v>
+      </c>
+      <c r="B28" s="1">
+        <v>-58.919377735300003</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F28" s="1">
+        <v>231.1937229088</v>
+      </c>
+      <c r="G28" s="1">
+        <v>-1.7209616038940001</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>265.72421484490002</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-58.886262831019998</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F29" s="1">
+        <v>265.72421484490002</v>
+      </c>
+      <c r="G29" s="1">
+        <v>-1.6709917948549999</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>305.4120910661</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-58.849622717560003</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F30" s="1">
+        <v>305.4120910661</v>
+      </c>
+      <c r="G30" s="1">
+        <v>-1.604009795471</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>351.02764504850001</v>
+      </c>
+      <c r="B31" s="1">
+        <v>-58.893899104239999</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F31" s="1">
+        <v>351.02764504850001</v>
+      </c>
+      <c r="G31" s="1">
+        <v>-1.670855240281</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>403.4562192944</v>
+      </c>
+      <c r="B32" s="1">
+        <v>-58.919302130029997</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F32" s="1">
+        <v>403.4562192944</v>
+      </c>
+      <c r="G32" s="1">
+        <v>-1.7592180654339999</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>463.71538875469997</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-58.832125359880003</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F33" s="1">
+        <v>463.71538875469997</v>
+      </c>
+      <c r="G33" s="1">
+        <v>-1.710310230141</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>532.97471072320002</v>
+      </c>
+      <c r="B34" s="1">
+        <v>-58.856492201800002</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F34" s="1">
+        <v>532.97471072320002</v>
+      </c>
+      <c r="G34" s="1">
+        <v>-1.612538125028</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>612.57842452320006</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-58.93686172196</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F35" s="1">
+        <v>612.57842452320006</v>
+      </c>
+      <c r="G35" s="1">
+        <v>-1.7171846446100001</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>704.07154155980004</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-58.870254753879998</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F36" s="1">
+        <v>704.07154155980004</v>
+      </c>
+      <c r="G36" s="1">
+        <v>-1.709932782481</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>809.22983211539997</v>
+      </c>
+      <c r="B37" s="1">
+        <v>-58.890530662659998</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F37" s="1">
+        <v>809.22983211539997</v>
+      </c>
+      <c r="G37" s="1">
+        <v>-1.688902099738</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>930.09429089369996</v>
+      </c>
+      <c r="B38" s="1">
+        <v>-58.88235843535</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F38" s="1">
+        <v>930.09429089369996</v>
+      </c>
+      <c r="G38" s="1">
+        <v>-1.6578238434879999</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1069.010750248</v>
+      </c>
+      <c r="B39" s="1">
+        <v>-58.9948989512</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1069.010750248</v>
+      </c>
+      <c r="G39" s="1">
+        <v>-1.703592630211</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1228.67540994</v>
+      </c>
+      <c r="B40" s="1">
+        <v>-58.922621120300001</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1228.67540994</v>
+      </c>
+      <c r="G40" s="1">
+        <v>-1.656603460376</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>1412.1871670989999</v>
+      </c>
+      <c r="B41" s="1">
+        <v>-58.956441476560002</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1412.1871670989999</v>
+      </c>
+      <c r="G41" s="1">
+        <v>-1.6053584558109999</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1623.107762053</v>
+      </c>
+      <c r="B42" s="1">
+        <v>-59.041407487500003</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1623.107762053</v>
+      </c>
+      <c r="G42" s="1">
+        <v>-1.6093526886730001</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1865.5309073870001</v>
+      </c>
+      <c r="B43" s="1">
+        <v>-58.929823931850002</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1865.5309073870001</v>
+      </c>
+      <c r="G43" s="1">
+        <v>-1.6966046443689999</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2144.1617419260001</v>
+      </c>
+      <c r="B44" s="1">
+        <v>-58.809818281440002</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2144.1617419260001</v>
+      </c>
+      <c r="G44" s="1">
+        <v>-1.734616277602</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2464.4081517660002</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-58.86013860245</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2464.4081517660002</v>
+      </c>
+      <c r="G45" s="1">
+        <v>-1.719578396035</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>2832.4857307819998</v>
+      </c>
+      <c r="B46" s="1">
+        <v>-58.936388750589998</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2832.4857307819998</v>
+      </c>
+      <c r="G46" s="1">
+        <v>-1.678917357799</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>3255.538417747</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-58.903401987670001</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3255.538417747</v>
+      </c>
+      <c r="G47" s="1">
+        <v>-1.646482821257</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>3741.7771515119998</v>
+      </c>
+      <c r="B48" s="1">
+        <v>-58.94959052467</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3741.7771515119998</v>
+      </c>
+      <c r="G48" s="1">
+        <v>-1.6205079104839999</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>4300.6392353580004</v>
+      </c>
+      <c r="B49" s="1">
+        <v>-58.93063789456</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F49" s="1">
+        <v>4300.6392353580004</v>
+      </c>
+      <c r="G49" s="1">
+        <v>-1.618845550633</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>4942.9715035890003</v>
+      </c>
+      <c r="B50" s="1">
+        <v>-58.908227694920001</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F50" s="1">
+        <v>4942.9715035890003</v>
+      </c>
+      <c r="G50" s="1">
+        <v>-1.632115167299</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>5681.2408454099996</v>
+      </c>
+      <c r="B51" s="1">
+        <v>-58.90190838174</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F51" s="1">
+        <v>5681.2408454099996</v>
+      </c>
+      <c r="G51" s="1">
+        <v>-1.6631504236779999</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>6529.7761721099996</v>
+      </c>
+      <c r="B52" s="1">
+        <v>-58.947029944640001</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F52" s="1">
+        <v>6529.7761721099996</v>
+      </c>
+      <c r="G52" s="1">
+        <v>-1.698178534667</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>7505.0465238249999</v>
+      </c>
+      <c r="B53" s="1">
+        <v>-58.91921682281</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F53" s="1">
+        <v>7505.0465238249999</v>
+      </c>
+      <c r="G53" s="1">
+        <v>-1.6502490219299999</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>8625.9807136060008</v>
+      </c>
+      <c r="B54" s="1">
+        <v>-58.930624470209999</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F54" s="1">
+        <v>8625.9807136060008</v>
+      </c>
+      <c r="G54" s="1">
+        <v>-1.6133367268679999</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
+        <v>15</v>
+      </c>
+      <c r="J54" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>9914.3347126869994</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-58.956429500500001</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F55" s="1">
+        <v>9914.3347126869994</v>
+      </c>
+      <c r="G55" s="1">
+        <v>-1.6301594027499999</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" t="s">
+        <v>15</v>
+      </c>
+      <c r="J55" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>11395.11390747</v>
+      </c>
+      <c r="B56" s="1">
+        <v>-58.97857133438</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F56" s="1">
+        <v>11395.11390747</v>
+      </c>
+      <c r="G56" s="1">
+        <v>-1.63053102505</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>13097.058423709999</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-58.993085028979998</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F57" s="1">
+        <v>13097.058423709999</v>
+      </c>
+      <c r="G57" s="1">
+        <v>-1.661069365103</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>15053.20093743</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-58.884482172360002</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F58" s="1">
+        <v>15053.20093743</v>
+      </c>
+      <c r="G58" s="1">
+        <v>-1.652785903679</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>15</v>
+      </c>
+      <c r="J58" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>17301.50779906</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-58.954894537400001</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F59" s="1">
+        <v>17301.50779906</v>
+      </c>
+      <c r="G59" s="1">
+        <v>-1.6636610678270001</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J59" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>19885.6159142</v>
+      </c>
+      <c r="B60" s="1">
+        <v>-58.964228736419997</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F60" s="1">
+        <v>19885.6159142</v>
+      </c>
+      <c r="G60" s="1">
+        <v>-1.626347431298</v>
+      </c>
+      <c r="H60" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>22855.67968293</v>
+      </c>
+      <c r="B61" s="1">
+        <v>-59.07153149637</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F61" s="1">
+        <v>22855.67968293</v>
+      </c>
+      <c r="G61" s="1">
+        <v>-1.706453154414</v>
+      </c>
+      <c r="H61" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" t="s">
+        <v>15</v>
+      </c>
+      <c r="J61" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>26269.34443583</v>
+      </c>
+      <c r="B62" s="1">
+        <v>-59.133931924979997</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F62" s="1">
+        <v>26269.34443583</v>
+      </c>
+      <c r="G62" s="1">
+        <v>-1.5925759798550001</v>
+      </c>
+      <c r="H62" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" t="s">
+        <v>15</v>
+      </c>
+      <c r="J62" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>30192.865259819999</v>
+      </c>
+      <c r="B63" s="1">
+        <v>-59.25963780611</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F63" s="1">
+        <v>30192.865259819999</v>
+      </c>
+      <c r="G63" s="1">
+        <v>-1.641477213555</v>
+      </c>
+      <c r="H63" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>34702.392928929999</v>
+      </c>
+      <c r="B64" s="1">
+        <v>-59.521359840640002</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F64" s="1">
+        <v>34702.392928929999</v>
+      </c>
+      <c r="G64" s="1">
+        <v>-1.6296163840789999</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>39885.451898359999</v>
+      </c>
+      <c r="B65" s="1">
+        <v>-59.704849681459997</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F65" s="1">
+        <v>39885.451898359999</v>
+      </c>
+      <c r="G65" s="1">
+        <v>-1.637250448112</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" t="s">
+        <v>15</v>
+      </c>
+      <c r="J65" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>45842.639047800003</v>
+      </c>
+      <c r="B66" s="1">
+        <v>-60.140916850460002</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45842.639047800003</v>
+      </c>
+      <c r="G66" s="1">
+        <v>-1.6710919231370001</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" t="s">
+        <v>15</v>
+      </c>
+      <c r="J66" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>52689.576144760002</v>
+      </c>
+      <c r="B67" s="1">
+        <v>-60.681313911140002</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F67" s="1">
+        <v>52689.576144760002</v>
+      </c>
+      <c r="G67" s="1">
+        <v>-1.558603170529</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" t="s">
+        <v>15</v>
+      </c>
+      <c r="J67" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>60559.153922619997</v>
+      </c>
+      <c r="B68" s="1">
+        <v>-60.666888976229998</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F68" s="1">
+        <v>60559.153922619997</v>
+      </c>
+      <c r="G68" s="1">
+        <v>-1.591478416001</v>
+      </c>
+      <c r="H68" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" t="s">
+        <v>15</v>
+      </c>
+      <c r="J68" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>69604.111328350002</v>
+      </c>
+      <c r="B69" s="1">
+        <v>-59.916402867670001</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F69" s="1">
+        <v>69604.111328350002</v>
+      </c>
+      <c r="G69" s="1">
+        <v>-1.602196848116</v>
+      </c>
+      <c r="H69" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B70" s="1">
+        <v>-58.112661602140001</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+      <c r="F70" s="1">
+        <v>80000</v>
+      </c>
+      <c r="G70" s="1">
+        <v>-1.6234360926339999</v>
+      </c>
+      <c r="H70" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" t="s">
+        <v>15</v>
+      </c>
+      <c r="J70" s="1">
+        <v>3.402823466385E+38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>

</xml_diff>